<commit_message>
another portion of functions
</commit_message>
<xml_diff>
--- a/out/dimension_1/d6/stat.xlsx
+++ b/out/dimension_1/d6/stat.xlsx
@@ -376,7 +376,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Statistic"/>
-  <dimension ref="A1:DF6"/>
+  <dimension ref="A1:DF8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1921,6 +1921,172 @@
       </c>
       <c r="DF6">
         <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>194700</v>
+      </c>
+      <c r="C7">
+        <v>251</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0.00796812749003984</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0.9920318725099602</v>
+      </c>
+      <c r="K7" t="str">
+        <v/>
+      </c>
+      <c r="L7" t="str">
+        <v/>
+      </c>
+      <c r="M7" t="str">
+        <v/>
+      </c>
+      <c r="N7" t="str">
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <v/>
+      </c>
+      <c r="Q7" t="str">
+        <v/>
+      </c>
+      <c r="R7" t="str">
+        <v/>
+      </c>
+      <c r="S7" t="str">
+        <v/>
+      </c>
+      <c r="T7" t="str">
+        <v/>
+      </c>
+      <c r="U7" t="str">
+        <v/>
+      </c>
+      <c r="V7" t="str">
+        <v/>
+      </c>
+      <c r="W7" t="str">
+        <v/>
+      </c>
+      <c r="X7" t="str">
+        <v/>
+      </c>
+      <c r="Y7" t="str">
+        <v/>
+      </c>
+      <c r="Z7" t="str">
+        <v/>
+      </c>
+      <c r="AA7" t="str">
+        <v/>
+      </c>
+      <c r="AB7" t="str">
+        <v/>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>194700</v>
+      </c>
+      <c r="C8">
+        <v>251</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0.00796812749003984</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0.9920318725099602</v>
+      </c>
+      <c r="K8" t="str">
+        <v/>
+      </c>
+      <c r="L8" t="str">
+        <v/>
+      </c>
+      <c r="M8" t="str">
+        <v/>
+      </c>
+      <c r="N8" t="str">
+        <v/>
+      </c>
+      <c r="O8" t="str">
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <v/>
+      </c>
+      <c r="Q8" t="str">
+        <v/>
+      </c>
+      <c r="R8" t="str">
+        <v/>
+      </c>
+      <c r="S8" t="str">
+        <v/>
+      </c>
+      <c r="T8" t="str">
+        <v/>
+      </c>
+      <c r="U8" t="str">
+        <v/>
+      </c>
+      <c r="V8" t="str">
+        <v/>
+      </c>
+      <c r="W8" t="str">
+        <v/>
+      </c>
+      <c r="X8" t="str">
+        <v/>
+      </c>
+      <c r="Y8" t="str">
+        <v/>
+      </c>
+      <c r="Z8" t="str">
+        <v/>
+      </c>
+      <c r="AA8" t="str">
+        <v/>
+      </c>
+      <c r="AB8" t="str">
+        <v/>
+      </c>
+      <c r="AC8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>